<commit_message>
update table and results Par config
</commit_message>
<xml_diff>
--- a/IBP_2018/Doc/res_Parameter_setting_runs.xlsx
+++ b/IBP_2018/Doc/res_Parameter_setting_runs.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="64">
   <si>
     <t>run</t>
   </si>
@@ -72,9 +72,6 @@
   </si>
   <si>
     <t>Cor.F</t>
-  </si>
-  <si>
-    <t>TUR.ctrl@f.vars["catch unique",]            &lt;- c(0,1,2,2,3,3,3,3,3)</t>
   </si>
   <si>
     <t>minor change in AIC You want to give as much freedom as possible</t>
@@ -597,8 +594,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -608,8 +605,9 @@
     <col min="3" max="3" width="9.88671875" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="11" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="4.44140625" customWidth="1"/>
     <col min="8" max="8" width="15.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="50.77734375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="37.6640625" customWidth="1"/>
     <col min="10" max="10" width="8" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="56.109375" bestFit="1" customWidth="1"/>
   </cols>
@@ -640,7 +638,7 @@
         <v>5</v>
       </c>
       <c r="J1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
@@ -671,7 +669,7 @@
       </c>
       <c r="J2" s="6"/>
       <c r="K2" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
@@ -765,9 +763,6 @@
       <c r="H6" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="I6" t="s">
-        <v>16</v>
-      </c>
       <c r="J6" s="7">
         <f t="shared" si="0"/>
         <v>1.2638000000000602</v>
@@ -802,7 +797,7 @@
       <c r="I8" s="6"/>
       <c r="J8" s="6"/>
       <c r="K8" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
@@ -858,7 +853,7 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B12" s="2">
         <v>1</v>
@@ -876,10 +871,10 @@
         <v>-0.3588982</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
@@ -899,7 +894,7 @@
         <v>-0.4401698</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J13">
         <f>$C$12-C13</f>
@@ -924,7 +919,7 @@
       </c>
       <c r="G14" s="5"/>
       <c r="H14" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I14" s="6"/>
       <c r="J14" s="6">
@@ -932,7 +927,7 @@
         <v>3.5710000000000264</v>
       </c>
       <c r="K14" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
@@ -943,7 +938,7 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B16" s="2">
         <v>1</v>
@@ -962,7 +957,7 @@
       </c>
       <c r="G16" s="2"/>
       <c r="H16" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I16" s="1"/>
     </row>
@@ -984,12 +979,12 @@
       </c>
       <c r="G17" s="5"/>
       <c r="H17" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I17" s="6"/>
       <c r="J17" s="6"/>
       <c r="K17" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.3">
@@ -1010,13 +1005,13 @@
       </c>
       <c r="G18" s="2"/>
       <c r="H18" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I18" s="2"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B20" s="2">
         <v>1</v>
@@ -1035,7 +1030,7 @@
       </c>
       <c r="G20" s="2"/>
       <c r="H20" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
@@ -1050,7 +1045,7 @@
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
       <c r="H21" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.3">
@@ -1071,7 +1066,7 @@
       </c>
       <c r="G22" s="2"/>
       <c r="H22" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.3">
@@ -1092,12 +1087,12 @@
       </c>
       <c r="G23" s="5"/>
       <c r="H23" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I23" s="6"/>
       <c r="J23" s="6"/>
       <c r="K23" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.3">
@@ -1118,7 +1113,7 @@
       </c>
       <c r="G24" s="2"/>
       <c r="H24" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.3">
@@ -1129,7 +1124,7 @@
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B26" s="2">
         <v>1</v>
@@ -1142,10 +1137,10 @@
       <c r="F26" s="2"/>
       <c r="G26" s="2"/>
       <c r="H26" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I26" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.3">
@@ -1166,10 +1161,10 @@
       </c>
       <c r="G27" s="2"/>
       <c r="H27" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I27" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.3">
@@ -1190,14 +1185,14 @@
       </c>
       <c r="G28" s="5"/>
       <c r="H28" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I28" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J28" s="6"/>
       <c r="K28" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.3">
@@ -1208,7 +1203,7 @@
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B30" s="2">
         <v>1</v>
@@ -1227,7 +1222,7 @@
       </c>
       <c r="G30" s="2"/>
       <c r="H30" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.3">
@@ -1248,10 +1243,10 @@
       </c>
       <c r="G31" s="5"/>
       <c r="H31" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I31" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J31" s="6">
         <f>C31-C28</f>
@@ -1277,7 +1272,7 @@
       </c>
       <c r="G32" s="2"/>
       <c r="H32" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J32">
         <v>0</v>
@@ -1285,7 +1280,7 @@
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B34" s="2">
         <v>1</v>
@@ -1304,7 +1299,7 @@
       </c>
       <c r="G34" s="2"/>
       <c r="H34" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I34" s="2"/>
     </row>
@@ -1326,7 +1321,7 @@
       </c>
       <c r="G35" s="2"/>
       <c r="H35" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J35">
         <f>C35-C34</f>
@@ -1351,22 +1346,22 @@
       </c>
       <c r="G36" s="6"/>
       <c r="H36" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I36" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J36" s="6">
         <f>C36-C34</f>
         <v>-4.438199999999938</v>
       </c>
       <c r="K36" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A38" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B38" s="3"/>
       <c r="C38" s="4"/>
@@ -1376,12 +1371,12 @@
       <c r="G38" s="4"/>
       <c r="H38" s="3"/>
       <c r="I38" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A39" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B39" s="2">
         <v>1</v>
@@ -1400,10 +1395,10 @@
       </c>
       <c r="G39" s="2"/>
       <c r="H39" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I39" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J39">
         <f>AVERAGE(D39:F39)</f>
@@ -1428,10 +1423,10 @@
       </c>
       <c r="G40" s="2"/>
       <c r="H40" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I40" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J40">
         <f>AVERAGE(D40:F40)</f>
@@ -1456,17 +1451,17 @@
       </c>
       <c r="G41" s="5"/>
       <c r="H41" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I41" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J41" s="6">
         <f t="shared" ref="J41:J43" si="1">AVERAGE(D41:F41)</f>
         <v>-2.1190226666666665</v>
       </c>
       <c r="K41" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.3">
@@ -1487,10 +1482,10 @@
       </c>
       <c r="G42" s="2"/>
       <c r="H42" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I42" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J42">
         <f t="shared" si="1"/>
@@ -1515,10 +1510,10 @@
       </c>
       <c r="G43" s="2"/>
       <c r="H43" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I43" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J43">
         <f>SUM(D43:F43)</f>

</xml_diff>

<commit_message>
Update report and final assessment
Update report and final assessment
</commit_message>
<xml_diff>
--- a/IBP_2018/Doc/res_Parameter_setting_runs.xlsx
+++ b/IBP_2018/Doc/res_Parameter_setting_runs.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="64">
   <si>
     <t>run</t>
   </si>
@@ -113,9 +113,6 @@
     <t>obs.vars BTS</t>
   </si>
   <si>
-    <t>cor.obs BTS</t>
-  </si>
-  <si>
     <t xml:space="preserve"> 0 0 0 0 0 </t>
   </si>
   <si>
@@ -194,9 +191,6 @@
     <t>uses less parameters</t>
   </si>
   <si>
-    <t xml:space="preserve"> failed</t>
-  </si>
-  <si>
     <t xml:space="preserve"> sum(MR) =-10.26, mean(MR)= -3.42</t>
   </si>
   <si>
@@ -216,6 +210,12 @@
   </si>
   <si>
     <t>sum(MR)=-6.84, mean(MR)= -2.28</t>
+  </si>
+  <si>
+    <t>lowest AIC, but additional parameter not estimated well</t>
+  </si>
+  <si>
+    <t>can estimate parameter</t>
   </si>
 </sst>
 </file>
@@ -238,17 +238,18 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Lucida Console"/>
       <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -265,7 +266,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -278,23 +280,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -309,10 +306,12 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="3">
-    <cellStyle name="Bad" xfId="2" builtinId="27"/>
+  <cellStyles count="2">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -592,15 +591,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K43"/>
+  <dimension ref="A1:K42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C41" sqref="C41"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="N36" sqref="N36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.88671875" style="2"/>
     <col min="3" max="3" width="9.88671875" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="11" bestFit="1" customWidth="1"/>
@@ -613,62 +612,64 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="G1" s="9"/>
+      <c r="H1" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="9" t="s">
         <v>17</v>
       </c>
+      <c r="K1" s="9"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="5">
+      <c r="B2" s="3">
         <v>1</v>
       </c>
-      <c r="C2" s="6">
+      <c r="C2" s="4">
         <v>883.12630000000001</v>
       </c>
-      <c r="D2" s="6">
+      <c r="D2" s="4">
         <v>-3.4187219999999998</v>
       </c>
-      <c r="E2" s="6">
+      <c r="E2" s="4">
         <v>-1.848522</v>
       </c>
-      <c r="F2" s="6">
+      <c r="F2" s="4">
         <v>4.1732310000000004</v>
       </c>
-      <c r="G2" s="6"/>
-      <c r="H2" s="5" t="s">
+      <c r="G2" s="4"/>
+      <c r="H2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="I2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="6"/>
-      <c r="K2" s="6" t="s">
+      <c r="J2" s="4"/>
+      <c r="K2" s="4" t="s">
         <v>16</v>
       </c>
     </row>
@@ -691,7 +692,7 @@
       <c r="H3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="J3" s="7">
+      <c r="J3" s="5">
         <f>$C$2-C3</f>
         <v>1.6796000000000504</v>
       </c>
@@ -715,7 +716,7 @@
       <c r="H4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="J4" s="7">
+      <c r="J4" s="5">
         <f t="shared" ref="J4:J6" si="0">$C$2-C4</f>
         <v>-2.4492000000000189</v>
       </c>
@@ -739,7 +740,7 @@
       <c r="H5" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="J5" s="7">
+      <c r="J5" s="5">
         <f t="shared" si="0"/>
         <v>-53.518100000000004</v>
       </c>
@@ -763,41 +764,41 @@
       <c r="H6" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="J6" s="7">
+      <c r="J6" s="5">
         <f t="shared" si="0"/>
         <v>1.2638000000000602</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="J7" s="7"/>
+      <c r="J7" s="5"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="5">
+      <c r="B8" s="3">
         <v>2</v>
       </c>
-      <c r="C8" s="6">
+      <c r="C8" s="4">
         <v>881.44669999999996</v>
       </c>
-      <c r="D8" s="6">
+      <c r="D8" s="4">
         <v>-4.7409840000000001</v>
       </c>
-      <c r="E8" s="6">
+      <c r="E8" s="4">
         <v>-1.4899960000000001</v>
       </c>
-      <c r="F8" s="6">
+      <c r="F8" s="4">
         <v>3.666423</v>
       </c>
-      <c r="G8" s="6"/>
-      <c r="H8" s="5">
+      <c r="G8" s="4"/>
+      <c r="H8" s="3">
         <v>2</v>
       </c>
-      <c r="I8" s="6"/>
-      <c r="J8" s="6"/>
-      <c r="K8" s="6" t="s">
-        <v>62</v>
+      <c r="I8" s="4"/>
+      <c r="J8" s="4"/>
+      <c r="K8" s="4" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
@@ -819,7 +820,7 @@
       <c r="H9" s="2">
         <v>0</v>
       </c>
-      <c r="J9" s="7">
+      <c r="J9" s="5">
         <f>$C$8-C9</f>
         <v>-25.871300000000019</v>
       </c>
@@ -843,13 +844,13 @@
       <c r="H10" s="2">
         <v>1</v>
       </c>
-      <c r="J10" s="7">
+      <c r="J10" s="5">
         <f>$C$8-C10</f>
         <v>-20.526100000000042</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="J11" s="7"/>
+      <c r="J11" s="5"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
@@ -874,7 +875,7 @@
         <v>21</v>
       </c>
       <c r="I12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
@@ -902,32 +903,32 @@
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B14" s="5">
+      <c r="B14" s="3">
         <v>3</v>
       </c>
-      <c r="C14" s="5">
+      <c r="C14" s="3">
         <v>875.95209999999997</v>
       </c>
-      <c r="D14" s="5">
+      <c r="D14" s="3">
         <v>-2.5709610000000001</v>
       </c>
-      <c r="E14" s="5">
+      <c r="E14" s="3">
         <v>-2.8560140000000001</v>
       </c>
-      <c r="F14" s="5">
+      <c r="F14" s="3">
         <v>-0.70433190000000001</v>
       </c>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5" t="s">
+      <c r="G14" s="3"/>
+      <c r="H14" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="I14" s="6"/>
-      <c r="J14" s="6">
+      <c r="I14" s="4"/>
+      <c r="J14" s="4">
         <f>$C$12-C14</f>
         <v>3.5710000000000264</v>
       </c>
-      <c r="K14" s="6" t="s">
-        <v>45</v>
+      <c r="K14" s="4" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
@@ -962,29 +963,29 @@
       <c r="I16" s="1"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B17" s="5">
+      <c r="B17" s="3">
         <v>2</v>
       </c>
-      <c r="C17" s="5">
+      <c r="C17" s="3">
         <v>875.95209999999997</v>
       </c>
-      <c r="D17" s="5">
+      <c r="D17" s="3">
         <v>-2.5709610000000001</v>
       </c>
-      <c r="E17" s="5">
+      <c r="E17" s="3">
         <v>-2.8560140000000001</v>
       </c>
-      <c r="F17" s="5">
+      <c r="F17" s="3">
         <v>-0.70433190000000001</v>
       </c>
-      <c r="G17" s="5"/>
-      <c r="H17" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="I17" s="6"/>
-      <c r="J17" s="6"/>
-      <c r="K17" s="8" t="s">
-        <v>47</v>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="I17" s="4"/>
+      <c r="J17" s="4"/>
+      <c r="K17" s="6" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.3">
@@ -1005,7 +1006,7 @@
       </c>
       <c r="G18" s="2"/>
       <c r="H18" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I18" s="2"/>
     </row>
@@ -1045,7 +1046,7 @@
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
       <c r="H21" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.3">
@@ -1066,33 +1067,33 @@
       </c>
       <c r="G22" s="2"/>
       <c r="H22" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B23" s="3">
+        <v>4</v>
+      </c>
+      <c r="C23" s="3">
+        <v>875.95209999999997</v>
+      </c>
+      <c r="D23" s="3">
+        <v>-2.5709610000000001</v>
+      </c>
+      <c r="E23" s="3">
+        <v>-2.8560140000000001</v>
+      </c>
+      <c r="F23" s="3">
+        <v>-0.70433190000000001</v>
+      </c>
+      <c r="G23" s="3"/>
+      <c r="H23" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="I23" s="4"/>
+      <c r="J23" s="4"/>
+      <c r="K23" s="4" t="s">
         <v>44</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B23" s="5">
-        <v>4</v>
-      </c>
-      <c r="C23" s="5">
-        <v>875.95209999999997</v>
-      </c>
-      <c r="D23" s="5">
-        <v>-2.5709610000000001</v>
-      </c>
-      <c r="E23" s="5">
-        <v>-2.8560140000000001</v>
-      </c>
-      <c r="F23" s="5">
-        <v>-0.70433190000000001</v>
-      </c>
-      <c r="G23" s="5"/>
-      <c r="H23" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="I23" s="6"/>
-      <c r="J23" s="6"/>
-      <c r="K23" s="6" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.3">
@@ -1113,7 +1114,7 @@
       </c>
       <c r="G24" s="2"/>
       <c r="H24" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.3">
@@ -1137,10 +1138,10 @@
       <c r="F26" s="2"/>
       <c r="G26" s="2"/>
       <c r="H26" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="I26" s="9" t="s">
-        <v>50</v>
+        <v>35</v>
+      </c>
+      <c r="I26" s="7" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.3">
@@ -1161,38 +1162,38 @@
       </c>
       <c r="G27" s="2"/>
       <c r="H27" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="I27" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="I27" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B28" s="3">
+        <v>3</v>
+      </c>
+      <c r="C28" s="3">
+        <v>875.95209999999997</v>
+      </c>
+      <c r="D28" s="3">
+        <v>-2.5709610000000001</v>
+      </c>
+      <c r="E28" s="3">
+        <v>-2.8560140000000001</v>
+      </c>
+      <c r="F28" s="3">
+        <v>-0.70433190000000001</v>
+      </c>
+      <c r="G28" s="3"/>
+      <c r="H28" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="I28" s="4" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B28" s="5">
-        <v>3</v>
-      </c>
-      <c r="C28" s="5">
-        <v>875.95209999999997</v>
-      </c>
-      <c r="D28" s="5">
-        <v>-2.5709610000000001</v>
-      </c>
-      <c r="E28" s="5">
-        <v>-2.8560140000000001</v>
-      </c>
-      <c r="F28" s="5">
-        <v>-0.70433190000000001</v>
-      </c>
-      <c r="G28" s="5"/>
-      <c r="H28" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="I28" s="6" t="s">
+      <c r="J28" s="4"/>
+      <c r="K28" s="4" t="s">
         <v>52</v>
-      </c>
-      <c r="J28" s="6"/>
-      <c r="K28" s="6" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.3">
@@ -1222,37 +1223,37 @@
       </c>
       <c r="G30" s="2"/>
       <c r="H30" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B31" s="5">
+      <c r="B31" s="3">
         <v>2</v>
       </c>
-      <c r="C31" s="5">
+      <c r="C31" s="3">
         <v>874.25139999999999</v>
       </c>
-      <c r="D31" s="5">
+      <c r="D31" s="3">
         <v>-2.4810599999999998</v>
       </c>
-      <c r="E31" s="5">
+      <c r="E31" s="3">
         <v>-3.0342889999999998</v>
       </c>
-      <c r="F31" s="5">
+      <c r="F31" s="3">
         <v>-0.80957060000000003</v>
       </c>
-      <c r="G31" s="5"/>
-      <c r="H31" s="5" t="s">
+      <c r="G31" s="3"/>
+      <c r="H31" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="I31" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="J31" s="6">
+      <c r="I31" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="J31" s="4">
         <f>C31-C28</f>
         <v>-1.7006999999999834</v>
       </c>
-      <c r="K31" s="6"/>
+      <c r="K31" s="4"/>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B32" s="2">
@@ -1272,7 +1273,7 @@
       </c>
       <c r="G32" s="2"/>
       <c r="H32" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J32">
         <v>0</v>
@@ -1299,7 +1300,7 @@
       </c>
       <c r="G34" s="2"/>
       <c r="H34" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I34" s="2"/>
     </row>
@@ -1321,7 +1322,7 @@
       </c>
       <c r="G35" s="2"/>
       <c r="H35" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J35">
         <f>C35-C34</f>
@@ -1329,194 +1330,182 @@
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B36" s="5">
+      <c r="B36" s="3">
         <v>3</v>
       </c>
-      <c r="C36" s="10">
+      <c r="C36" s="8">
         <v>872.28430000000003</v>
       </c>
-      <c r="D36" s="10">
+      <c r="D36" s="8">
         <v>-2.5378470000000002</v>
       </c>
-      <c r="E36" s="10">
+      <c r="E36" s="8">
         <v>-3.0732919999999999</v>
       </c>
-      <c r="F36" s="10">
+      <c r="F36" s="8">
         <v>-0.71718020000000005</v>
       </c>
-      <c r="G36" s="6"/>
-      <c r="H36" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="I36" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="J36" s="6">
+      <c r="G36" s="4"/>
+      <c r="H36" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="I36" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="J36" s="4">
         <f>C36-C34</f>
         <v>-4.438199999999938</v>
       </c>
-      <c r="K36" s="6" t="s">
-        <v>45</v>
+      <c r="K36" s="4" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A38" s="4" t="s">
+      <c r="A38" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B38" s="3">
+        <v>1</v>
+      </c>
+      <c r="C38" s="8">
+        <v>865.11239999999998</v>
+      </c>
+      <c r="D38" s="8">
+        <v>-2.5613600000000001</v>
+      </c>
+      <c r="E38" s="8">
+        <v>-2.1063589999999999</v>
+      </c>
+      <c r="F38" s="8">
+        <v>-5.592911</v>
+      </c>
+      <c r="G38" s="4"/>
+      <c r="H38" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B38" s="3"/>
-      <c r="C38" s="4"/>
-      <c r="D38" s="4"/>
-      <c r="E38" s="4"/>
-      <c r="F38" s="4"/>
-      <c r="G38" s="4"/>
-      <c r="H38" s="3"/>
       <c r="I38" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
+      </c>
+      <c r="J38" s="4">
+        <f>AVERAGE(D38:F38)</f>
+        <v>-3.4202099999999995</v>
+      </c>
+      <c r="K38" s="4" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A39" s="9" t="s">
-        <v>31</v>
-      </c>
       <c r="B39" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C39" s="2">
-        <v>865.11239999999998</v>
+        <v>866.14459999999997</v>
       </c>
       <c r="D39" s="2">
-        <v>-2.5613600000000001</v>
+        <v>-2.7094900000000002</v>
       </c>
       <c r="E39" s="2">
-        <v>-2.1063589999999999</v>
+        <v>-2.0796559999999999</v>
       </c>
       <c r="F39" s="2">
-        <v>-5.592911</v>
+        <v>-4.16493</v>
       </c>
       <c r="G39" s="2"/>
       <c r="H39" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="I39" s="7" t="s">
-        <v>57</v>
+        <v>41</v>
+      </c>
+      <c r="I39" s="5" t="s">
+        <v>56</v>
       </c>
       <c r="J39">
         <f>AVERAGE(D39:F39)</f>
-        <v>-3.4202099999999995</v>
+        <v>-2.9846920000000003</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B40" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C40" s="2">
-        <v>866.14459999999997</v>
+        <v>862.93989999999997</v>
       </c>
       <c r="D40" s="2">
-        <v>-2.7094900000000002</v>
+        <v>-2.406806</v>
       </c>
       <c r="E40" s="2">
-        <v>-2.0796559999999999</v>
+        <v>-2.1685500000000002</v>
       </c>
       <c r="F40" s="2">
-        <v>-4.16493</v>
+        <v>-1.781712</v>
       </c>
       <c r="G40" s="2"/>
       <c r="H40" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="I40" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="J40">
+        <f t="shared" ref="J40:J41" si="1">AVERAGE(D40:F40)</f>
+        <v>-2.1190226666666665</v>
+      </c>
+      <c r="K40" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B41" s="2">
+        <v>4</v>
+      </c>
+      <c r="C41" s="2">
+        <v>864.90830000000005</v>
+      </c>
+      <c r="D41" s="2">
+        <v>-2.394228</v>
+      </c>
+      <c r="E41" s="2">
+        <v>-2.1950409999999998</v>
+      </c>
+      <c r="F41" s="2">
+        <v>-1.6854830000000001</v>
+      </c>
+      <c r="G41" s="2"/>
+      <c r="H41" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="I40" s="7" t="s">
+      <c r="I41" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="J40">
-        <f>AVERAGE(D40:F40)</f>
-        <v>-2.9846920000000003</v>
-      </c>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B41" s="5">
-        <v>3</v>
-      </c>
-      <c r="C41" s="5">
-        <v>862.93989999999997</v>
-      </c>
-      <c r="D41" s="5">
-        <v>-2.406806</v>
-      </c>
-      <c r="E41" s="5">
-        <v>-2.1685500000000002</v>
-      </c>
-      <c r="F41" s="5">
-        <v>-1.781712</v>
-      </c>
-      <c r="G41" s="5"/>
-      <c r="H41" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="I41" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="J41" s="6">
-        <f t="shared" ref="J41:J43" si="1">AVERAGE(D41:F41)</f>
-        <v>-2.1190226666666665</v>
-      </c>
-      <c r="K41" s="6" t="s">
-        <v>45</v>
+      <c r="J41">
+        <f t="shared" si="1"/>
+        <v>-2.0915839999999997</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B42" s="2">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C42" s="2">
-        <v>864.90830000000005</v>
+        <v>863.57330000000002</v>
       </c>
       <c r="D42" s="2">
-        <v>-2.394228</v>
+        <v>-2.3208690000000001</v>
       </c>
       <c r="E42" s="2">
-        <v>-2.1950409999999998</v>
+        <v>-2.572489</v>
       </c>
       <c r="F42" s="2">
-        <v>-1.6854830000000001</v>
+        <v>-1.9417709999999999</v>
       </c>
       <c r="G42" s="2"/>
       <c r="H42" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="I42" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
+      </c>
+      <c r="I42" s="5" t="s">
+        <v>61</v>
       </c>
       <c r="J42">
-        <f t="shared" si="1"/>
-        <v>-2.0915839999999997</v>
-      </c>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B43" s="2">
-        <v>5</v>
-      </c>
-      <c r="C43" s="2">
-        <v>863.57330000000002</v>
-      </c>
-      <c r="D43" s="2">
-        <v>-2.3208690000000001</v>
-      </c>
-      <c r="E43" s="2">
-        <v>-2.572489</v>
-      </c>
-      <c r="F43" s="2">
-        <v>-1.9417709999999999</v>
-      </c>
-      <c r="G43" s="2"/>
-      <c r="H43" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="I43" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="J43">
-        <f>SUM(D43:F43)</f>
+        <f>SUM(D42:F42)</f>
         <v>-6.8351290000000002</v>
       </c>
     </row>

</xml_diff>